<commit_message>
missing class due to capitalization of 'Of' in 'End of Day' while checking menu name
</commit_message>
<xml_diff>
--- a/src/test/resources/inventory_data/InventoryData.xlsx
+++ b/src/test/resources/inventory_data/InventoryData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Load" sheetId="4" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="27">
   <si>
     <t>Item Code</t>
   </si>
@@ -83,22 +83,25 @@
     <t>5</t>
   </si>
   <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>28002.08</t>
-  </si>
-  <si>
     <t>52.08</t>
   </si>
   <si>
-    <t>25</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
     <t>18000</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>7842.08</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>19</t>
   </si>
 </sst>
 </file>
@@ -501,7 +504,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -1186,7 +1189,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -1209,7 +1212,7 @@
         <v>17</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1217,7 +1220,7 @@
         <v>16</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1225,7 +1228,7 @@
         <v>100</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1241,7 +1244,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1249,7 +1252,7 @@
         <v>13</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1257,7 +1260,7 @@
         <v>14</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1265,7 +1268,7 @@
         <v>15</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>